<commit_message>
corrected parse error for port-channels
</commit_message>
<xml_diff>
--- a/Terraform/aci/migrate-configs/143b-core01_export.xlsx
+++ b/Terraform/aci/migrate-configs/143b-core01_export.xlsx
@@ -2705,7 +2705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>Ethernet1/7</t>
+          <t>Ethernet1/8</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
@@ -3502,12 +3502,12 @@
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>169,811-812,3960,3963,3965-3967</t>
+          <t>1-994,997,999-4094</t>
         </is>
       </c>
       <c r="M10" s="2" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="Q10" s="2" t="inlineStr">
         <is>
-          <t>asgard-leaf-vpc</t>
+          <t>r143b-ucs-b-vpc</t>
         </is>
       </c>
       <c r="R10" s="2" t="inlineStr"/>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Ethernet1/8</t>
+          <t>Ethernet1/21</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
@@ -3582,12 +3582,12 @@
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>21</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="L11" s="3" t="inlineStr">
         <is>
-          <t>1-994,997,999-4094</t>
+          <t>64</t>
         </is>
       </c>
       <c r="M11" s="3" t="inlineStr">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="Q11" s="3" t="inlineStr">
         <is>
-          <t>r143b-ucs-b-vpc</t>
+          <t>142b-oob-vpc</t>
         </is>
       </c>
       <c r="R11" s="3" t="inlineStr"/>
@@ -3652,7 +3652,7 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Ethernet1/21</t>
+          <t>Ethernet1/27</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr">
@@ -3662,12 +3662,12 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>27</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
@@ -3687,7 +3687,7 @@
       </c>
       <c r="L12" s="2" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>169,811-812,3960,3963,3965-3967</t>
         </is>
       </c>
       <c r="M12" s="2" t="inlineStr">
@@ -3712,10 +3712,14 @@
       </c>
       <c r="Q12" s="2" t="inlineStr">
         <is>
-          <t>142b-oob-vpc</t>
-        </is>
-      </c>
-      <c r="R12" s="2" t="inlineStr"/>
+          <t>asgard-leaf-vpc</t>
+        </is>
+      </c>
+      <c r="R12" s="2" t="inlineStr">
+        <is>
+          <t>asgard-leaf101-Eth1/49</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
@@ -3732,7 +3736,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Ethernet1/21</t>
+          <t>Ethernet1/28</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
@@ -3742,12 +3746,12 @@
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>27</t>
         </is>
       </c>
       <c r="I13" s="3" t="inlineStr">
@@ -3757,7 +3761,7 @@
       </c>
       <c r="J13" s="3" t="inlineStr">
         <is>
-          <t>access</t>
+          <t>trunk</t>
         </is>
       </c>
       <c r="K13" s="3" t="inlineStr">
@@ -3767,7 +3771,7 @@
       </c>
       <c r="L13" s="3" t="inlineStr">
         <is>
-          <t>n/a</t>
+          <t>169,811-812,3960,3963,3965-3967</t>
         </is>
       </c>
       <c r="M13" s="3" t="inlineStr">
@@ -3792,10 +3796,14 @@
       </c>
       <c r="Q13" s="3" t="inlineStr">
         <is>
-          <t>r143c-netapp01-ct0-vpc</t>
-        </is>
-      </c>
-      <c r="R13" s="3" t="inlineStr"/>
+          <t>asgard-leaf-vpc</t>
+        </is>
+      </c>
+      <c r="R13" s="3" t="inlineStr">
+        <is>
+          <t>asgard-leaf102-Eth1/49</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
@@ -3812,7 +3820,7 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Ethernet1/27</t>
+          <t>Ethernet1/29</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr">
@@ -3822,12 +3830,12 @@
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H14" s="2" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I14" s="2" t="inlineStr">
@@ -3847,7 +3855,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>169,811-812,3960,3963,3965-3967</t>
+          <t>168,812,3910,3961-3962,3964</t>
         </is>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -3872,14 +3880,10 @@
       </c>
       <c r="Q14" s="2" t="inlineStr">
         <is>
-          <t>asgard-leaf-vpc</t>
-        </is>
-      </c>
-      <c r="R14" s="2" t="inlineStr">
-        <is>
-          <t>asgard-leaf101-Eth1/49</t>
-        </is>
-      </c>
+          <t>wakanda-leaf-vpc</t>
+        </is>
+      </c>
+      <c r="R14" s="2" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -3896,7 +3900,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Ethernet1/28</t>
+          <t>Ethernet1/30</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -3906,12 +3910,12 @@
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
@@ -3931,7 +3935,7 @@
       </c>
       <c r="L15" s="3" t="inlineStr">
         <is>
-          <t>169,811-812,3960,3963,3965-3967</t>
+          <t>168,812,3910,3961-3962,3964</t>
         </is>
       </c>
       <c r="M15" s="3" t="inlineStr">
@@ -3956,14 +3960,10 @@
       </c>
       <c r="Q15" s="3" t="inlineStr">
         <is>
-          <t>asgard-leaf-vpc</t>
-        </is>
-      </c>
-      <c r="R15" s="3" t="inlineStr">
-        <is>
-          <t>asgard-leaf102-Eth1/49</t>
-        </is>
-      </c>
+          <t>wakanda-leaf-vpc</t>
+        </is>
+      </c>
+      <c r="R15" s="3" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
@@ -3980,7 +3980,7 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Ethernet1/29</t>
+          <t>Ethernet1/31</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr">
@@ -3990,12 +3990,12 @@
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I16" s="2" t="inlineStr">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="L16" s="2" t="inlineStr">
         <is>
-          <t>168,812,3910,3961-3962,3964</t>
+          <t>1-994,997,1000-3966,3968-4094</t>
         </is>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="Q16" s="2" t="inlineStr">
         <is>
-          <t>wakanda-leaf-vpc</t>
+          <t>143-oob-vpc</t>
         </is>
       </c>
       <c r="R16" s="2" t="inlineStr"/>
@@ -4060,7 +4060,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>Ethernet1/30</t>
+          <t>Ethernet1/32</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
@@ -4070,12 +4070,12 @@
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
@@ -4095,7 +4095,7 @@
       </c>
       <c r="L17" s="3" t="inlineStr">
         <is>
-          <t>168,812,3910,3961-3962,3964</t>
+          <t>1-994,997,1000-3966,3968-4094</t>
         </is>
       </c>
       <c r="M17" s="3" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="Q17" s="3" t="inlineStr">
         <is>
-          <t>wakanda-leaf-vpc</t>
+          <t>143-oob-vpc</t>
         </is>
       </c>
       <c r="R17" s="3" t="inlineStr"/>
@@ -4140,7 +4140,7 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Ethernet1/31</t>
+          <t>Ethernet1/33</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
@@ -4150,12 +4150,12 @@
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>33</t>
         </is>
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>33</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr">
@@ -4200,7 +4200,7 @@
       </c>
       <c r="Q18" s="2" t="inlineStr">
         <is>
-          <t>143-oob-vpc</t>
+          <t>143-dist-vpc</t>
         </is>
       </c>
       <c r="R18" s="2" t="inlineStr"/>
@@ -4220,7 +4220,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>Ethernet1/32</t>
+          <t>Ethernet1/34</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
@@ -4230,12 +4230,12 @@
       </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>33</t>
         </is>
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>33</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="Q19" s="3" t="inlineStr">
         <is>
-          <t>143-oob-vpc</t>
+          <t>143-dist-vpc</t>
         </is>
       </c>
       <c r="R19" s="3" t="inlineStr"/>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Ethernet1/33</t>
+          <t>Ethernet1/35</t>
         </is>
       </c>
       <c r="F20" s="2" t="inlineStr">
@@ -4310,12 +4310,12 @@
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>peer-link</t>
         </is>
       </c>
       <c r="I20" s="2" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>1-994,997,1000-3966,3968-4094</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="M20" s="2" t="inlineStr">
@@ -4360,10 +4360,14 @@
       </c>
       <c r="Q20" s="2" t="inlineStr">
         <is>
-          <t>143-dist-vpc</t>
-        </is>
-      </c>
-      <c r="R20" s="2" t="inlineStr"/>
+          <t>Peer-Link - Core</t>
+        </is>
+      </c>
+      <c r="R20" s="2" t="inlineStr">
+        <is>
+          <t>143c-core02-Eth1/35</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
@@ -4380,7 +4384,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Ethernet1/34</t>
+          <t>Ethernet1/36</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
@@ -4390,12 +4394,12 @@
       </c>
       <c r="G21" s="3" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>peer-link</t>
         </is>
       </c>
       <c r="I21" s="3" t="inlineStr">
@@ -4415,7 +4419,7 @@
       </c>
       <c r="L21" s="3" t="inlineStr">
         <is>
-          <t>1-994,997,1000-3966,3968-4094</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="M21" s="3" t="inlineStr">
@@ -4440,174 +4444,10 @@
       </c>
       <c r="Q21" s="3" t="inlineStr">
         <is>
-          <t>143-dist-vpc</t>
-        </is>
-      </c>
-      <c r="R21" s="3" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>intf_add</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr"/>
-      <c r="C22" s="2" t="inlineStr"/>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>143b-core01</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>Ethernet1/35</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>vpc</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>peer-link</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>9216</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>trunk</t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L22" s="2" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="M22" s="2" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N22" s="2" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="O22" s="2" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="P22" s="2" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="Q22" s="2" t="inlineStr">
-        <is>
           <t>Peer-Link - Core</t>
         </is>
       </c>
-      <c r="R22" s="2" t="inlineStr">
-        <is>
-          <t>143c-core02-Eth1/35</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>intf_add</t>
-        </is>
-      </c>
-      <c r="B23" s="3" t="inlineStr"/>
-      <c r="C23" s="3" t="inlineStr"/>
-      <c r="D23" s="3" t="inlineStr">
-        <is>
-          <t>143b-core01</t>
-        </is>
-      </c>
-      <c r="E23" s="3" t="inlineStr">
-        <is>
-          <t>Ethernet1/36</t>
-        </is>
-      </c>
-      <c r="F23" s="3" t="inlineStr">
-        <is>
-          <t>vpc</t>
-        </is>
-      </c>
-      <c r="G23" s="3" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="H23" s="3" t="inlineStr">
-        <is>
-          <t>peer-link</t>
-        </is>
-      </c>
-      <c r="I23" s="3" t="inlineStr">
-        <is>
-          <t>9216</t>
-        </is>
-      </c>
-      <c r="J23" s="3" t="inlineStr">
-        <is>
-          <t>trunk</t>
-        </is>
-      </c>
-      <c r="K23" s="3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L23" s="3" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="M23" s="3" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N23" s="3" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="O23" s="3" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="P23" s="3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="Q23" s="3" t="inlineStr">
-        <is>
-          <t>Peer-Link - Core</t>
-        </is>
-      </c>
-      <c r="R23" s="3" t="inlineStr">
+      <c r="R21" s="3" t="inlineStr">
         <is>
           <t>143c-core02-Eth1/36</t>
         </is>

</xml_diff>

<commit_message>
added best practices from unoffical aci guide
</commit_message>
<xml_diff>
--- a/Terraform/aci/migrate-configs/143b-core01_export.xlsx
+++ b/Terraform/aci/migrate-configs/143b-core01_export.xlsx
@@ -681,7 +681,11 @@
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
-      <c r="C2" s="2" t="inlineStr"/>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">v0001_bd
@@ -702,7 +706,11 @@
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr"/>
-      <c r="C3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>intersite</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
           <t>v0056_bd</t>
@@ -727,7 +735,11 @@
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr"/>
-      <c r="C4" s="2" t="inlineStr"/>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
           <t>v0064_bd</t>
@@ -752,7 +764,11 @@
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr"/>
-      <c r="C5" s="3" t="inlineStr"/>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
           <t>v0080_bd</t>
@@ -777,7 +793,11 @@
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr"/>
-      <c r="C6" s="2" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">v0087_bd
@@ -798,7 +818,11 @@
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr"/>
-      <c r="C7" s="3" t="inlineStr"/>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
           <t>v0090_bd</t>
@@ -823,7 +847,11 @@
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr"/>
-      <c r="C8" s="2" t="inlineStr"/>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
           <t>v0091_bd</t>
@@ -848,7 +876,11 @@
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr"/>
-      <c r="C9" s="3" t="inlineStr"/>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
           <t>v0110_bd</t>
@@ -873,7 +905,11 @@
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr"/>
-      <c r="C10" s="2" t="inlineStr"/>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">v0136_bd
@@ -894,7 +930,11 @@
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr"/>
-      <c r="C11" s="3" t="inlineStr"/>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
           <t>v0168_bd</t>
@@ -919,7 +959,11 @@
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr"/>
-      <c r="C12" s="2" t="inlineStr"/>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
           <t>v0169_bd</t>
@@ -944,7 +988,11 @@
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr"/>
-      <c r="C13" s="3" t="inlineStr"/>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
           <t>v0691_bd</t>
@@ -969,7 +1017,11 @@
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr"/>
-      <c r="C14" s="2" t="inlineStr"/>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>v0811_bd</t>
@@ -994,7 +1046,11 @@
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr"/>
-      <c r="C15" s="3" t="inlineStr"/>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
           <t>v0812_bd</t>
@@ -1019,7 +1075,11 @@
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr"/>
-      <c r="C16" s="2" t="inlineStr"/>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>v0995_bd</t>
@@ -1044,7 +1104,11 @@
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr"/>
-      <c r="C17" s="3" t="inlineStr"/>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
           <t>v0996_bd</t>
@@ -1069,7 +1133,11 @@
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr"/>
-      <c r="C18" s="2" t="inlineStr"/>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
           <t>v0997_bd</t>
@@ -1094,7 +1162,11 @@
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr"/>
-      <c r="C19" s="3" t="inlineStr"/>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
           <t>v0998_bd</t>
@@ -1119,7 +1191,11 @@
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr"/>
-      <c r="C20" s="2" t="inlineStr"/>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
           <t>v0999_bd</t>
@@ -1144,7 +1220,11 @@
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr"/>
-      <c r="C21" s="3" t="inlineStr"/>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">v3001_bd
@@ -1165,7 +1245,11 @@
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr"/>
-      <c r="C22" s="2" t="inlineStr"/>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">v3003_bd
@@ -1186,7 +1270,11 @@
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr"/>
-      <c r="C23" s="3" t="inlineStr"/>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
           <t>v3004_bd</t>
@@ -1211,7 +1299,11 @@
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr"/>
-      <c r="C24" s="2" t="inlineStr"/>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">v3006_bd
@@ -1232,7 +1324,11 @@
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr"/>
-      <c r="C25" s="3" t="inlineStr"/>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">v3007_bd
@@ -1253,7 +1349,11 @@
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr"/>
-      <c r="C26" s="2" t="inlineStr"/>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">v3011_bd
@@ -1274,7 +1374,11 @@
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr"/>
-      <c r="C27" s="3" t="inlineStr"/>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">v3019_bd
@@ -1295,7 +1399,11 @@
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr"/>
-      <c r="C28" s="2" t="inlineStr"/>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
           <t>v3103_bd</t>
@@ -1320,7 +1428,11 @@
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr"/>
-      <c r="C29" s="3" t="inlineStr"/>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
           <t>v3910_bd</t>
@@ -1345,7 +1457,11 @@
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr"/>
-      <c r="C30" s="2" t="inlineStr"/>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
           <t>v3960_bd</t>
@@ -1370,7 +1486,11 @@
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr"/>
-      <c r="C31" s="3" t="inlineStr"/>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
           <t>v3961_bd</t>
@@ -1395,7 +1515,11 @@
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr"/>
-      <c r="C32" s="2" t="inlineStr"/>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
           <t>v3962_bd</t>
@@ -1420,7 +1544,11 @@
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr"/>
-      <c r="C33" s="3" t="inlineStr"/>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
           <t>v3963_bd</t>
@@ -1445,7 +1573,11 @@
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr"/>
-      <c r="C34" s="2" t="inlineStr"/>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
           <t>v3964_bd</t>
@@ -1470,7 +1602,11 @@
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr"/>
-      <c r="C35" s="3" t="inlineStr"/>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
           <t>v3965_bd</t>
@@ -1495,7 +1631,11 @@
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr"/>
-      <c r="C36" s="2" t="inlineStr"/>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
           <t>v3966_bd</t>
@@ -1520,7 +1660,11 @@
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr"/>
-      <c r="C37" s="3" t="inlineStr"/>
+      <c r="C37" s="3" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
       <c r="D37" s="3" t="inlineStr">
         <is>
           <t>v3967_bd</t>

</xml_diff>